<commit_message>
POM with Page Factory fifth
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\seleniumworkspaces\LiveProjects\PageObjectwithFactories\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17205" windowHeight="5370" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SignInTest" sheetId="1" r:id="rId1"/>
     <sheet name="FlightSearchTest" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Y</t>
   </si>
@@ -39,50 +34,44 @@
     <t>password</t>
   </si>
   <si>
-    <t>trainer@way2automation.com</t>
-  </si>
-  <si>
-    <t>Selenium@123</t>
-  </si>
-  <si>
-    <t>java@way2automation.com</t>
-  </si>
-  <si>
-    <t>Delhi, India (DEL-Indira Gandhi Intl.)</t>
-  </si>
-  <si>
     <t>fromCity</t>
   </si>
   <si>
     <t>toCity</t>
   </si>
   <si>
-    <t>Seattle, WA, United States (SEA-Seattle - Tacoma Intl.)</t>
-  </si>
-  <si>
     <t>fromDate</t>
   </si>
   <si>
     <t>toDate</t>
   </si>
   <si>
-    <t>14/12/2017</t>
-  </si>
-  <si>
-    <t>noOfAdults</t>
-  </si>
-  <si>
-    <t>noOfChildern</t>
-  </si>
-  <si>
-    <t>N</t>
+    <t>ramesh.sanjay@gmail.com</t>
+  </si>
+  <si>
+    <t>Selenium@1234</t>
+  </si>
+  <si>
+    <t>uip311977@gmail.com</t>
+  </si>
+  <si>
+    <t>Bengaluru, India (BLR-Kempegowda Intl.)</t>
+  </si>
+  <si>
+    <t>Goa, India (GOI-Dabolim)</t>
+  </si>
+  <si>
+    <t>20/2/2020</t>
+  </si>
+  <si>
+    <t>26/2/2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -220,7 +209,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -397,23 +386,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -424,95 +417,82 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="7:7">
+      <c r="G21" s="1"/>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>43081</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>